<commit_message>
added all the tests
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9e094f0b9fd54ec/CodeBase/C^M^M/L2/S2/ASD2/MathsPourInfo2/MathsPourInfo2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:40000_{D96CEA82-7D1D-41B1-9D29-753108192293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="10_ncr:40000_{D96CEA82-7D1D-41B1-9D29-753108192293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B821BC-33DB-43D9-8F4A-6F2FBCB268B4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Model</t>
   </si>
@@ -42,9 +42,6 @@
     <t>1 (surface)</t>
   </si>
   <si>
-    <t>2 (surface + chambres</t>
-  </si>
-  <si>
     <t>3 (surface + chambres + salles de bain)</t>
   </si>
   <si>
@@ -58,12 +55,18 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2 (surface + chambres)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,8 +96,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,11 +417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,49 +433,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>75633.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>76932.800000000003</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41292.699999999997</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
         <v>74845.7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>75894.7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>39144.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
         <v>74845.3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>75894.600000000006</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39137.699999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>74565.600000000006</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the testing data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9e094f0b9fd54ec/CodeBase/C^M^M/L2/S2/ASD2/MathsPourInfo2/MathsPourInfo2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="10_ncr:40000_{D96CEA82-7D1D-41B1-9D29-753108192293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B821BC-33DB-43D9-8F4A-6F2FBCB268B4}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="14_{18A786CF-9336-41CA-980D-E98BD2F7992D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70CCDF82-5D9F-4FF7-9CF6-4B6EB39031DB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -48,19 +48,22 @@
     <t>4 (surface + chambres + salles de bain + type de propriété)</t>
   </si>
   <si>
-    <t>Seulement copropriétés</t>
-  </si>
-  <si>
-    <t>Seulement Individuelles</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>2 (surface + chambres)</t>
+  </si>
+  <si>
+    <t>Propriétées : seulement copropriétées</t>
+  </si>
+  <si>
+    <t>Propriétées : toutes</t>
+  </si>
+  <si>
+    <t>Propriétées : seulement individuelles</t>
+  </si>
+  <si>
+    <t>Moyenne :</t>
   </si>
 </sst>
 </file>
@@ -418,18 +421,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -437,13 +440,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -462,7 +465,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>74845.7</v>
@@ -496,10 +499,27 @@
         <v>74565.600000000006</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE(B2:B5)</f>
+        <v>74972.450000000012</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C2:C4)</f>
+        <v>76240.7</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE(D2:D4)</f>
+        <v>39858.433333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>